<commit_message>
upload bang gia kc l2
</commit_message>
<xml_diff>
--- a/DIAMOND_PRICE BY KIETNORMAL.xlsx
+++ b/DIAMOND_PRICE BY KIETNORMAL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DIAMOND_SHOP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{346A7C04-03B4-434E-B927-93EF6ABDF9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C269251-7251-4E6E-B977-B3E8E83466D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9764346E-DED0-479C-9BC2-6316E2CFFDDC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>Gồm Các Tiêu Chí:</t>
   </si>
@@ -81,13 +81,139 @@
   </si>
   <si>
     <t>Trọng lượng vỏ (Metal Weight): Khối lượng vỏ kim cương.(G)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bảng Giá Viên Kim Cương </t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Carat Weight (ct)</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Clarity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Cut</t>
+  </si>
+  <si>
+    <t>Price/Carat (VND)</t>
+  </si>
+  <si>
+    <t>Natural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0.5 - 1.0</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>Lab-grown</t>
+  </si>
+  <si>
+    <t>0.5 - 1.0</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>VS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Very Good</t>
+  </si>
+  <si>
+    <t>1.0 - 2.0</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>SI2</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>VS2</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>SI1</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Bảng giá vỏ kim cương</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Metal Weight (g)</t>
+  </si>
+  <si>
+    <t>Price (VND)</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Simple</t>
+  </si>
+  <si>
+    <t>Sliver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Complex</t>
+  </si>
+  <si>
+    <t>Platinum</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Complex</t>
+  </si>
+  <si>
+    <t>Bảng Tiền Công</t>
+  </si>
+  <si>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t>Labor Cost (VND)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +245,26 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +295,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -315,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,33 +473,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -376,30 +525,63 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F577610-EC77-4247-933B-50377606E0AE}">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,192 +940,489 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="22" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="16" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="23" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="22" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="19" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="21"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="19" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W11" s="1"/>
     </row>
     <row r="12" spans="1:23" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25"/>
     </row>
     <row r="13" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="3" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="3" t="s">
+      <c r="A15" s="30"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="19" spans="1:1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+    </row>
+    <row r="18" spans="1:16" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A18" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="J18" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="O18" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="P18" s="32"/>
+    </row>
+    <row r="19" spans="1:16" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="M19" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="P19" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="37">
+        <v>300000000</v>
+      </c>
+      <c r="J20" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="L20" s="42">
+        <v>3</v>
+      </c>
+      <c r="M20" s="43">
+        <v>6000000</v>
+      </c>
+      <c r="O20" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="P20" s="43">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="35"/>
+      <c r="E21" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="37">
+        <v>130000000</v>
+      </c>
+      <c r="J21" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="L21" s="42">
+        <v>5</v>
+      </c>
+      <c r="M21" s="43">
+        <v>9600000</v>
+      </c>
+      <c r="O21" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="P21" s="43">
+        <v>7200000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="35"/>
+      <c r="E22" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="37">
+        <v>90000000</v>
+      </c>
+      <c r="J22" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="K22" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" s="42">
+        <v>5</v>
+      </c>
+      <c r="M22" s="43">
+        <v>17000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A23" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="35"/>
+      <c r="E23" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="37">
+        <v>120000000</v>
+      </c>
+      <c r="J23" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="L23" s="42">
+        <v>8</v>
+      </c>
+      <c r="M23" s="43">
+        <v>7800000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A24" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="35"/>
+      <c r="E24" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="37">
+        <v>145000000</v>
+      </c>
+      <c r="J24" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="K24" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="L24" s="42">
+        <v>8</v>
+      </c>
+      <c r="M24" s="43">
+        <v>21000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A25" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="35"/>
+      <c r="E25" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="37">
+        <v>205000000</v>
+      </c>
+      <c r="J25" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="42">
+        <v>10</v>
+      </c>
+      <c r="M25" s="43">
+        <v>15600000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
     </row>
-    <row r="29" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:16" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="33">
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:B15"/>
+    <mergeCell ref="C15:F15"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:B9"/>
     <mergeCell ref="C2:J2"/>
@@ -955,11 +1434,6 @@
     <mergeCell ref="D6:J6"/>
     <mergeCell ref="D7:J7"/>
     <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:B15"/>
-    <mergeCell ref="C15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
upload bang gia kc final
</commit_message>
<xml_diff>
--- a/DIAMOND_PRICE BY KIETNORMAL.xlsx
+++ b/DIAMOND_PRICE BY KIETNORMAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C269251-7251-4E6E-B977-B3E8E83466D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63243792-6F40-4E75-92DB-E7CE7C980C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9764346E-DED0-479C-9BC2-6316E2CFFDDC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>Gồm Các Tiêu Chí:</t>
   </si>
@@ -207,13 +207,27 @@
   </si>
   <si>
     <t>Labor Cost (VND)</t>
+  </si>
+  <si>
+    <t>Công thức tính giá bán</t>
+  </si>
+  <si>
+    <t>Giá Vốn Sản phẩm:
+Giá Vốn Sản Phẩm =Giá Viên Kim Cương  +Giá Vỏ Kim Cương +Tiền Công</t>
+  </si>
+  <si>
+    <t>Giá Bán:
+Giá Bán=Giá Vốn Sản Phẩm*Tỉ lệ Áp Giá</t>
+  </si>
+  <si>
+    <t>Giá Viên Kim Cương =Price/Carat *Carat Weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +277,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +321,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -465,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -473,8 +505,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -525,63 +614,24 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F577610-EC77-4247-933B-50377606E0AE}">
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18:P21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,467 +990,548 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="12" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="21" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
     </row>
     <row r="5" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="15" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
     </row>
     <row r="6" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="22" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="21" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
     </row>
     <row r="8" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="18" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="41"/>
     </row>
     <row r="9" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="18" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="41"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W11" s="1"/>
     </row>
     <row r="12" spans="1:23" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="23" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="23" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="23" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="18" spans="1:16" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="J18" s="32" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="J18" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="O18" s="32" t="s">
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="O18" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="P18" s="32"/>
+      <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:16" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34" t="s">
+      <c r="D19" s="14"/>
+      <c r="E19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="34" t="s">
+      <c r="J19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K19" s="34" t="s">
+      <c r="K19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L19" s="34" t="s">
+      <c r="L19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M19" s="34" t="s">
+      <c r="M19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="O19" s="34" t="s">
+      <c r="O19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="P19" s="34" t="s">
+      <c r="P19" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36" t="s">
+      <c r="D20" s="11"/>
+      <c r="E20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="37">
+      <c r="H20" s="5">
         <v>300000000</v>
       </c>
-      <c r="J20" s="41" t="s">
+      <c r="J20" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K20" s="41" t="s">
+      <c r="K20" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="L20" s="42">
+      <c r="L20" s="8">
         <v>3</v>
       </c>
-      <c r="M20" s="43">
+      <c r="M20" s="9">
         <v>6000000</v>
       </c>
-      <c r="O20" s="42" t="s">
+      <c r="O20" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="P20" s="43">
+      <c r="P20" s="9">
         <v>3600000</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="35" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="36" t="s">
+      <c r="D21" s="11"/>
+      <c r="E21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21" s="5">
         <v>130000000</v>
       </c>
-      <c r="J21" s="41" t="s">
+      <c r="J21" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="K21" s="41" t="s">
+      <c r="K21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="L21" s="42">
+      <c r="L21" s="8">
         <v>5</v>
       </c>
-      <c r="M21" s="43">
+      <c r="M21" s="9">
         <v>9600000</v>
       </c>
-      <c r="O21" s="42" t="s">
+      <c r="O21" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="P21" s="43">
+      <c r="P21" s="9">
         <v>7200000</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35" t="s">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36" t="s">
+      <c r="D22" s="11"/>
+      <c r="E22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="36" t="s">
+      <c r="G22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="37">
+      <c r="H22" s="5">
         <v>90000000</v>
       </c>
-      <c r="J22" s="41" t="s">
+      <c r="J22" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K22" s="41" t="s">
+      <c r="K22" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="L22" s="42">
+      <c r="L22" s="8">
         <v>5</v>
       </c>
-      <c r="M22" s="43">
+      <c r="M22" s="9">
         <v>17000000</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36" t="s">
+      <c r="D23" s="11"/>
+      <c r="E23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="36" t="s">
+      <c r="G23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="37">
+      <c r="H23" s="5">
         <v>120000000</v>
       </c>
-      <c r="J23" s="41" t="s">
+      <c r="J23" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="L23" s="42">
+      <c r="L23" s="8">
         <v>8</v>
       </c>
-      <c r="M23" s="43">
+      <c r="M23" s="9">
         <v>7800000</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36" t="s">
+      <c r="D24" s="11"/>
+      <c r="E24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="36" t="s">
+      <c r="G24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="37">
+      <c r="H24" s="5">
         <v>145000000</v>
       </c>
-      <c r="J24" s="41" t="s">
+      <c r="J24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K24" s="41" t="s">
+      <c r="K24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L24" s="42">
+      <c r="L24" s="8">
         <v>8</v>
       </c>
-      <c r="M24" s="43">
+      <c r="M24" s="9">
         <v>21000000</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="35" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36" t="s">
+      <c r="D25" s="11"/>
+      <c r="E25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="36" t="s">
+      <c r="F25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="37">
+      <c r="H25" s="5">
         <v>205000000</v>
       </c>
-      <c r="J25" s="41" t="s">
+      <c r="J25" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K25" s="41" t="s">
+      <c r="K25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L25" s="42">
+      <c r="L25" s="8">
         <v>10</v>
       </c>
-      <c r="M25" s="43">
+      <c r="M25" s="9">
         <v>15600000</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
     </row>
-    <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:16" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:16" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A28" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+    </row>
+    <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+    </row>
+    <row r="30" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="46"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+    </row>
+    <row r="31" spans="1:16" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+    </row>
+    <row r="32" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="47"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="49"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+    </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="37">
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A29:F30"/>
+    <mergeCell ref="A31:F32"/>
+    <mergeCell ref="A33:F34"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:B9"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:B15"/>
+    <mergeCell ref="C15:F15"/>
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="C24:D24"/>
@@ -1417,23 +1548,6 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:B15"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:B9"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="C4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>